<commit_message>
moved model files to zenodo
</commit_message>
<xml_diff>
--- a/input/estimation_results_splineGC_distVoT_knots2040_2.xlsx
+++ b/input/estimation_results_splineGC_distVoT_knots2040_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="31">
   <si>
     <t>Value</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>.4E</t>
+  </si>
+  <si>
+    <t>Active bound</t>
   </si>
   <si>
     <t>mu_pt</t>
@@ -501,22 +504,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.079053355330598</v>
+        <v>-1.672980411206608</v>
       </c>
       <c r="C2">
-        <v>0.2737290037719375</v>
+        <v>0.09837465124506885</v>
       </c>
       <c r="D2">
-        <v>-18.55504270772237</v>
+        <v>-17.00621440617781</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.4460234816774667</v>
+        <v>0.06698565495354158</v>
       </c>
       <c r="G2">
-        <v>-11.38741246588317</v>
+        <v>-24.97520420404811</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -527,22 +530,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.153089616137727</v>
+        <v>-3.172365362002692</v>
       </c>
       <c r="C3">
-        <v>0.036778692294472</v>
+        <v>0.03681075798972867</v>
       </c>
       <c r="D3">
-        <v>-58.54176649073913</v>
+        <v>-86.18038680126824</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.04289859677874345</v>
+        <v>0.04271409608001418</v>
       </c>
       <c r="G3">
-        <v>-50.19021081837803</v>
+        <v>-74.26975291856952</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -553,25 +556,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-8.649330748413272</v>
+        <v>-5.277640166565115</v>
       </c>
       <c r="C4">
-        <v>0.3522962372672611</v>
+        <v>0.0805875730929403</v>
       </c>
       <c r="D4">
-        <v>-24.55130039283294</v>
+        <v>-65.489503703983</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1.949775717391839</v>
+        <v>0.09208822978042321</v>
       </c>
       <c r="G4">
-        <v>-4.436064451547916</v>
+        <v>-57.31069192174954</v>
       </c>
       <c r="H4">
-        <v>9.161842749794147E-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -579,22 +582,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.75467087097471</v>
+        <v>-2.185409835006344</v>
       </c>
       <c r="C5">
-        <v>0.02506935393331568</v>
+        <v>0.02221264413057192</v>
       </c>
       <c r="D5">
-        <v>-109.882004869456</v>
+        <v>-98.38584826551553</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.02726959231478546</v>
+        <v>0.02240191401144809</v>
       </c>
       <c r="G5">
-        <v>-101.0162102599949</v>
+        <v>-97.55460332048101</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -605,22 +608,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-1.854882070405445</v>
+        <v>-2.141938405479834</v>
       </c>
       <c r="C6">
-        <v>0.03291669004035929</v>
+        <v>0.03123343502117985</v>
       </c>
       <c r="D6">
-        <v>-56.3508076945515</v>
+        <v>-68.57838095705306</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.04095503826972707</v>
+        <v>0.03446794297528731</v>
       </c>
       <c r="G6">
-        <v>-45.29069313009352</v>
+        <v>-62.14291369274786</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -631,22 +634,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.4893294000890667</v>
+        <v>0.4432421580893682</v>
       </c>
       <c r="C7">
-        <v>0.04253597681167959</v>
+        <v>0.04219750733705776</v>
       </c>
       <c r="D7">
-        <v>11.50389474433571</v>
+        <v>10.50398912307585</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.05008808457797823</v>
+        <v>0.04928817490155355</v>
       </c>
       <c r="G7">
-        <v>9.769377372122664</v>
+        <v>8.992870175750761</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -657,22 +660,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.3349194118319121</v>
+        <v>-0.1395972114561939</v>
       </c>
       <c r="C8">
-        <v>0.005406073272844876</v>
+        <v>0.001777925369090756</v>
       </c>
       <c r="D8">
-        <v>-61.95243662608833</v>
+        <v>-78.5169129610794</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.01490721694176866</v>
+        <v>0.004603949987866079</v>
       </c>
       <c r="G8">
-        <v>-22.4669308255318</v>
+        <v>-30.32118329349986</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -691,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>102779</v>
+        <v>85518</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -707,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>-199630.7415369735</v>
+        <v>-166084.3154390672</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -718,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>-53190.05315635816</v>
+        <v>-53448.43018347587</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -729,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>292881.3767612307</v>
+        <v>225271.7705111827</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -740,7 +743,7 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.7335578040393801</v>
+        <v>0.6781849626066287</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -751,7 +754,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.7335227392996205</v>
+        <v>0.6781428153395525</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -762,7 +765,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>106394.1063127163</v>
+        <v>106910.8603669517</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -773,7 +776,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>106460.8886670332</v>
+        <v>106976.3557420653</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -784,7 +787,7 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>4235.072146578354</v>
+        <v>4323.442828912963</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -805,244 +808,271 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.242583913070618</v>
+        <v>-3.818346844050863</v>
       </c>
       <c r="C2">
-        <v>0.2655587225226765</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-19.74171235374483</v>
+        <v>0.2120296909587497</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-18.00854789150129</v>
       </c>
       <c r="F2">
-        <v>0.4374062634499782</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>-11.98561692217322</v>
+        <v>0.2313566295003963</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-16.50416005928338</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.115939708703271</v>
+        <v>-3.466486729244421</v>
       </c>
       <c r="C3">
-        <v>0.03490719401320067</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-60.61615000916709</v>
+        <v>0.04148964468080995</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-83.55064874411329</v>
       </c>
       <c r="F3">
-        <v>0.03973177069560602</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-53.25561060225475</v>
+        <v>0.05483186862407576</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-63.22029170682583</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-4.692038116676313</v>
+        <v>-5.28412159530715</v>
       </c>
       <c r="C4">
-        <v>0.07045002536775058</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-66.60094289794472</v>
+        <v>0.09594694784847523</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-55.07336829152846</v>
       </c>
       <c r="F4">
-        <v>0.1023620963735014</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-45.83765165922245</v>
+        <v>0.1457321159920942</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-36.25914273826784</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.920181395993504</v>
+        <v>-2.345845308152982</v>
       </c>
       <c r="C5">
-        <v>0.02701054665281872</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-108.1126359095278</v>
+        <v>0.02371545650574094</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-98.91630412364653</v>
       </c>
       <c r="F5">
-        <v>0.0352655458460635</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-82.80550678955301</v>
+        <v>0.02361237688598294</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-99.34812236313029</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.448750421865104</v>
+        <v>-3.009508142249753</v>
       </c>
       <c r="C6">
-        <v>0.03256518510426368</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-75.19534785461714</v>
+        <v>0.03621806063523202</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-83.09412733497328</v>
       </c>
       <c r="F6">
-        <v>0.03585337179548144</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-68.29902737833203</v>
+        <v>0.0516124311368935</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-58.30975359923517</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.5346388726203636</v>
+        <v>0.7157367362274738</v>
       </c>
       <c r="C7">
-        <v>0.04059303611969482</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>13.17070423222098</v>
+        <v>0.04292927515119934</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>16.67246264248833</v>
       </c>
       <c r="F7">
-        <v>0.04659868966629106</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>11.47325979440823</v>
+        <v>0.0517604712542244</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>13.8278635971472</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.3754760678502786</v>
+        <v>-0.1530319204208467</v>
       </c>
       <c r="C8">
-        <v>0.006402991809238544</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-58.64072281156501</v>
+        <v>0.002531391830031983</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-60.45366766428777</v>
       </c>
       <c r="F8">
-        <v>0.02054176043416986</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-18.27867037265701</v>
+        <v>0.003762704536853997</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-40.67072471993695</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>1.47299298349823</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.02950523232561442</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>49.92311083141271</v>
+        <v>0.01933613189491461</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>51.71665178095931</v>
       </c>
       <c r="F9">
-        <v>0.05198167846475723</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>28.33677224364535</v>
+        <v>0.03387254133351017</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>29.52243795804887</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1050,15 +1080,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>102779</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>85518</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1066,45 +1096,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-199630.7415369735</v>
+        <v>-166084.3154390672</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-40072.79462114612</v>
+        <v>-42154.94698063081</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>319115.8938316548</v>
+        <v>247858.7369168728</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7992654121673728</v>
+        <v>0.7461834558598246</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1115,7 +1145,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7992253381790762</v>
+        <v>0.7461352875545946</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1126,7 +1156,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>80161.58924229223</v>
+        <v>84325.89396126162</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1137,7 +1167,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>80237.91193294007</v>
+        <v>84400.74581853428</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1148,7 +1178,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.4937045894228351</v>
+        <v>672.3742929258788</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1203,25 +1233,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-12.57927279757805</v>
+        <v>-5.562167911462441</v>
       </c>
       <c r="C2">
-        <v>1.442692864510338</v>
+        <v>1.009460206027704</v>
       </c>
       <c r="D2">
-        <v>-8.719300626642775</v>
+        <v>-5.510041780992988</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3.58748535322917E-08</v>
       </c>
       <c r="F2">
-        <v>2.535212462603755</v>
+        <v>1.041649137950775</v>
       </c>
       <c r="G2">
-        <v>-4.961821931349567</v>
+        <v>-5.339771050360426</v>
       </c>
       <c r="H2">
-        <v>6.983500455692848E-07</v>
+        <v>9.306403381259543E-08</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1229,22 +1259,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.517761931690257</v>
+        <v>-3.874770466325772</v>
       </c>
       <c r="C3">
-        <v>0.07644369972184073</v>
+        <v>0.08682543877342253</v>
       </c>
       <c r="D3">
-        <v>-32.93616008711974</v>
+        <v>-44.62713371869361</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.09037972066226874</v>
+        <v>0.1176308202507108</v>
       </c>
       <c r="G3">
-        <v>-27.85759806780814</v>
+        <v>-32.94009561497007</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1255,22 +1285,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.998948215021476</v>
+        <v>-6.18365992631436</v>
       </c>
       <c r="C4">
-        <v>0.2034554030727224</v>
+        <v>0.2321505306114727</v>
       </c>
       <c r="D4">
-        <v>-29.48532270178753</v>
+        <v>-26.63642383253191</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.2987759138913925</v>
+        <v>0.3134747229252904</v>
       </c>
       <c r="G4">
-        <v>-20.0784197657986</v>
+        <v>-19.72618356149914</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1281,22 +1311,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-4.280572966406576</v>
+        <v>-3.398805984487677</v>
       </c>
       <c r="C5">
-        <v>0.09522904438277266</v>
+        <v>0.07045698869847988</v>
       </c>
       <c r="D5">
-        <v>-44.95028795207516</v>
+        <v>-48.23944433720889</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.1339969801057347</v>
+        <v>0.0731178725682626</v>
       </c>
       <c r="G5">
-        <v>-31.94529431207217</v>
+        <v>-46.48392882758675</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1307,22 +1337,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.320097257195292</v>
+        <v>-2.99092739968023</v>
       </c>
       <c r="C6">
-        <v>0.06796137318150966</v>
+        <v>0.06938404315058853</v>
       </c>
       <c r="D6">
-        <v>-34.13846937728628</v>
+        <v>-43.10684797063257</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.08253162167206009</v>
+        <v>0.09781299543488969</v>
       </c>
       <c r="G6">
-        <v>-28.11161601082084</v>
+        <v>-30.57801661611697</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1333,22 +1363,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.9464341683426422</v>
+        <v>1.186767499615756</v>
       </c>
       <c r="C7">
-        <v>0.08365825492126765</v>
+        <v>0.08435977603813884</v>
       </c>
       <c r="D7">
-        <v>11.31309957676441</v>
+        <v>14.06793089492345</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.09785068143739073</v>
+        <v>0.1067343984295755</v>
       </c>
       <c r="G7">
-        <v>9.672228690080338</v>
+        <v>11.11888498063535</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1359,22 +1389,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.5852478010659288</v>
+        <v>-0.1426630346561793</v>
       </c>
       <c r="C8">
-        <v>0.01980478755015943</v>
+        <v>0.004867241824864233</v>
       </c>
       <c r="D8">
-        <v>-29.55082449552545</v>
+        <v>-29.31085813887185</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.04399539004579339</v>
+        <v>0.009703332617792557</v>
       </c>
       <c r="G8">
-        <v>-13.30248011113808</v>
+        <v>-14.70247803260754</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1382,25 +1412,25 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>1.281829617005471</v>
+        <v>1.017374512202527</v>
       </c>
       <c r="C9">
-        <v>0.05191614148517699</v>
+        <v>0.03580135398466828</v>
       </c>
       <c r="D9">
-        <v>24.69038684955925</v>
+        <v>28.41720770220622</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.08067821186563318</v>
+        <v>0.05234822034042511</v>
       </c>
       <c r="G9">
-        <v>15.88817584529904</v>
+        <v>19.43474879540221</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1419,7 +1449,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>25456</v>
+        <v>22973</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1427,7 +1457,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>77323</v>
+        <v>62545</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1435,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-49430.88289479075</v>
+        <v>-44610.59514499285</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1446,7 +1476,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-10398.13381080171</v>
+        <v>-11326.9880144851</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -1457,7 +1487,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>78065.49816797808</v>
+        <v>66567.2142610155</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1468,7 +1498,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7896429680826617</v>
+        <v>0.7460919770814478</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1479,7 +1509,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7894811259400273</v>
+        <v>0.7459126474855524</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1490,7 +1520,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>20812.26762160343</v>
+        <v>22669.9760289702</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1501,7 +1531,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>20877.42527560805</v>
+        <v>22734.31262810854</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1512,7 +1542,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.06989141832003772</v>
+        <v>0.1506166934773418</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1533,244 +1563,271 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-8.955476910402302</v>
+        <v>-7.233566997328035</v>
       </c>
       <c r="C2">
-        <v>8.419780078431415</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-1.063623613322533</v>
+        <v>9.713305320796357</v>
       </c>
       <c r="E2">
-        <v>0.2874992409092616</v>
+        <v>-0.7447070547489989</v>
       </c>
       <c r="F2">
-        <v>0.6902809130190966</v>
+        <v>0.4564488334233063</v>
       </c>
       <c r="G2">
-        <v>-12.97367019933021</v>
+        <v>0.1914988489903077</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-37.77342284545087</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.7821312420556779</v>
+        <v>-0.4618166150392248</v>
       </c>
       <c r="C3">
-        <v>0.08862005940949388</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>8.825668220798867</v>
+        <v>0.0851710807783144</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-5.422223257225697</v>
       </c>
       <c r="F3">
-        <v>0.08324334887368347</v>
+        <v>5.886230058926856E-08</v>
       </c>
       <c r="G3">
-        <v>9.395720530687836</v>
+        <v>0.09424677693644623</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-4.900078602694745</v>
+      </c>
+      <c r="I3">
+        <v>9.579832092043716E-07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-1.972249767559213</v>
+        <v>-3.11288913405289</v>
       </c>
       <c r="C4">
-        <v>0.1863857290198558</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-10.58154923089153</v>
+        <v>0.2699019422146252</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-11.5334076832153</v>
       </c>
       <c r="F4">
-        <v>0.2098698693931764</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-9.397488897581303</v>
+        <v>0.3827514835838884</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-8.132925063817895</v>
+      </c>
+      <c r="I4">
+        <v>4.440892098500626E-16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.148743521394048</v>
+        <v>-1.122447474876091</v>
       </c>
       <c r="C5">
-        <v>0.1073936024827552</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-20.008114745374</v>
+        <v>0.07636771751165398</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-14.69793142246004</v>
       </c>
       <c r="F5">
-        <v>0.1089136587246704</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-19.72887098418014</v>
+        <v>0.06794155557354124</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-16.52077974077489</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-0.03948385916599839</v>
+        <v>-0.8404783913427564</v>
       </c>
       <c r="C6">
-        <v>0.09362110009833154</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-0.4217410297948641</v>
+        <v>0.09213149164789218</v>
       </c>
       <c r="E6">
-        <v>0.6732140528484218</v>
+        <v>-9.122596153711413</v>
       </c>
       <c r="F6">
-        <v>0.1050616482358499</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-0.3758161025359339</v>
+        <v>0.1259856593745364</v>
       </c>
       <c r="H6">
-        <v>0.7070536158162879</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-6.67122270515044</v>
+      </c>
+      <c r="I6">
+        <v>2.536815202347498E-11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.3989835771630851</v>
+        <v>0.6230555544287325</v>
       </c>
       <c r="C7">
-        <v>0.1083506232127586</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>3.682337630671825</v>
+        <v>0.1034534501122434</v>
       </c>
       <c r="E7">
-        <v>0.0002311050593166719</v>
+        <v>6.022569124110783</v>
       </c>
       <c r="F7">
-        <v>0.1024620859149093</v>
+        <v>1.716700115395042E-09</v>
       </c>
       <c r="G7">
-        <v>3.893963055704576</v>
+        <v>0.1062863986339531</v>
       </c>
       <c r="H7">
-        <v>9.861967590119036E-05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>5.862044085005792</v>
+      </c>
+      <c r="I7">
+        <v>4.572035861016843E-09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.6611563689280745</v>
+        <v>-0.1605231608246017</v>
       </c>
       <c r="C8">
-        <v>0.02960307672381965</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-22.33404233946012</v>
+        <v>0.007533943685942933</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-21.30665790933781</v>
       </c>
       <c r="F8">
-        <v>0.04361866585213115</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-15.15764767243039</v>
+        <v>0.01173981340637617</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-13.67339967579193</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>1.371892522239247</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.07858211600746379</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>17.45807560220119</v>
+        <v>0.05016420477456989</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>19.93453308975681</v>
       </c>
       <c r="F9">
-        <v>0.09976802026068353</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>13.75082434887085</v>
+        <v>0.07510141093945774</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>13.31532906626934</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1778,61 +1835,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>4448</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>98331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>81825</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-8634.598001221319</v>
+        <v>-7168.673002960919</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-3520.962970297772</v>
+        <v>-4196.470925158025</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>10227.27006184709</v>
+        <v>5944.404155605787</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.5922261847280267</v>
+        <v>0.4146097996903008</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1843,7 +1900,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.5912996795220091</v>
+        <v>0.4134938330397512</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1854,7 +1911,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>7057.925940595544</v>
+        <v>8408.94185031605</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1865,7 +1922,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>7109.127619282987</v>
+        <v>8458.65540563487</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1876,7 +1933,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.01652200441587012</v>
+        <v>22.95556482222339</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1897,244 +1954,271 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-10.4113220432118</v>
+        <v>-5.15428519278747</v>
       </c>
       <c r="C2">
-        <v>1.20566253855523</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-8.635353351600278</v>
+        <v>1.030869407664259</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-4.999940006432079</v>
       </c>
       <c r="F2">
-        <v>1.657289561448085</v>
+        <v>5.734815577973507E-07</v>
       </c>
       <c r="G2">
-        <v>-6.282138188401266</v>
+        <v>1.063478147455382</v>
       </c>
       <c r="H2">
-        <v>3.339477583352846E-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-4.84663009307741</v>
+      </c>
+      <c r="I2">
+        <v>1.255762537732963E-06</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.821322997213516</v>
+        <v>-4.087511920259394</v>
       </c>
       <c r="C3">
-        <v>0.09480676045746923</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-29.7586689345764</v>
+        <v>0.1088970626018388</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-37.53555718214913</v>
       </c>
       <c r="F3">
-        <v>0.1108420559742094</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-25.45354263250023</v>
+        <v>0.1401789229288025</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-29.15924758770947</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-6.973135746052662</v>
+        <v>-6.895030542932053</v>
       </c>
       <c r="C4">
-        <v>0.3244192306316546</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-21.49421208007843</v>
+        <v>0.3634403564761442</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-18.97156003748482</v>
       </c>
       <c r="F4">
-        <v>0.5857101401912821</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-11.90543797615552</v>
+        <v>0.524275958647925</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-13.15152913117341</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.242033702144538</v>
+        <v>-2.258752699669295</v>
       </c>
       <c r="C5">
-        <v>0.05854085225507595</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-55.3807055629845</v>
+        <v>0.04975895003499979</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-45.39389794359644</v>
       </c>
       <c r="F5">
-        <v>0.05983350399332543</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-54.18425273081441</v>
+        <v>0.04642912899257431</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-48.64947391174516</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-3.141614457710157</v>
+        <v>-3.753755439077343</v>
       </c>
       <c r="C6">
-        <v>0.08898783979637061</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-35.30386247041238</v>
+        <v>0.09876368824433451</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-38.00744490010147</v>
       </c>
       <c r="F6">
-        <v>0.1041476545714085</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-30.16500439341261</v>
+        <v>0.1454000558498358</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-25.81674000836763</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.8084365707380931</v>
+        <v>0.9905134710247595</v>
       </c>
       <c r="C7">
-        <v>0.1100873327928647</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>7.343593038621531</v>
+        <v>0.1165443909943353</v>
       </c>
       <c r="E7">
-        <v>2.078337502098293E-13</v>
+        <v>8.499023098184999</v>
       </c>
       <c r="F7">
-        <v>0.1303980003941175</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>6.199762023149575</v>
+        <v>0.1438286446706847</v>
       </c>
       <c r="H7">
-        <v>5.654861023884905E-10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>6.88676079297469</v>
+      </c>
+      <c r="I7">
+        <v>5.70765656959793E-12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.6001986051752259</v>
+        <v>-0.2620702823242717</v>
       </c>
       <c r="C8">
-        <v>0.01630782475932133</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-36.80433252338946</v>
+        <v>0.01143039230226287</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-22.92749674675556</v>
       </c>
       <c r="F8">
-        <v>0.0239637996843865</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-25.04605334212848</v>
+        <v>0.01803292406051982</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-14.53287783194475</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>1.779453097910451</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.1028563140962734</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>17.30037784792566</v>
+        <v>0.04870775357144485</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>20.53061220598469</v>
       </c>
       <c r="F9">
-        <v>0.1543426355231638</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>11.5292387737113</v>
+        <v>0.09497672273616414</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>10.52889561980255</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2142,61 +2226,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>28751</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>21284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>74028</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>64234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-55855.60549303455</v>
+        <v>-41338.59721782148</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-6865.294049635911</v>
+        <v>-7020.168444799745</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>97980.62288679728</v>
+        <v>68636.85754604347</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8770885394753791</v>
+        <v>0.8301788421167499</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2207,7 +2291,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8769453130269433</v>
+        <v>0.8299853183752972</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2218,7 +2302,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>13746.58809927182</v>
+        <v>14056.33688959949</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2229,7 +2313,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>13812.71952189766</v>
+        <v>14120.06257676522</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2240,7 +2324,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.1362894753144417</v>
+        <v>177.9766714558397</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -2261,244 +2345,271 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-3.019291090391079</v>
+        <v>-2.56527896921774</v>
       </c>
       <c r="C2">
-        <v>0.2764006337658846</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-10.92360407881142</v>
+        <v>0.2975998408780923</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-8.619893618385944</v>
       </c>
       <c r="F2">
-        <v>0.2913819233833061</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>-10.36197117286261</v>
+        <v>0.3684566167393651</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-6.962227987433159</v>
+      </c>
+      <c r="I2">
+        <v>3.349320820689172E-12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.781281202456023</v>
+        <v>-4.552613433800848</v>
       </c>
       <c r="C3">
-        <v>0.1483588074205712</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-18.74699083129982</v>
+        <v>0.2786932846654471</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-16.33556918770382</v>
       </c>
       <c r="F3">
-        <v>0.1647102482718615</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-16.88590255698842</v>
+        <v>0.4041507488752643</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-11.26464183592531</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-3.526058029459032</v>
+        <v>-5.770148450447874</v>
       </c>
       <c r="C4">
-        <v>0.2139885207715612</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-16.47779056907075</v>
+        <v>0.5620648929450079</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-10.265982670105</v>
       </c>
       <c r="F4">
-        <v>0.2696266353485552</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-13.07755824976557</v>
+        <v>0.8711637915431425</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-6.623494349124496</v>
+      </c>
+      <c r="I4">
+        <v>3.508060508750077E-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.158867744332425</v>
+        <v>-3.603596977143348</v>
       </c>
       <c r="C5">
-        <v>0.1558499023902698</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-20.26865397979</v>
+        <v>0.1751034577406484</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-20.57981620489047</v>
       </c>
       <c r="F5">
-        <v>0.1516737667156288</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-20.82672444111542</v>
+        <v>0.2352023450792066</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-15.32126295734765</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.808644510267398</v>
+        <v>-3.481006697370505</v>
       </c>
       <c r="C6">
-        <v>0.1354095237081426</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-20.74185355175654</v>
+        <v>0.1897212314789268</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-18.34800812874313</v>
       </c>
       <c r="F6">
-        <v>0.1407709560735629</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-19.95187493647256</v>
+        <v>0.2607918969731022</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-13.34783303382134</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.7339479740678994</v>
+        <v>0.8858946781004471</v>
       </c>
       <c r="C7">
-        <v>0.1733044307976432</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>4.235021405337782</v>
+        <v>0.2013991355605487</v>
       </c>
       <c r="E7">
-        <v>2.285299359106041E-05</v>
+        <v>4.398701492112966</v>
       </c>
       <c r="F7">
-        <v>0.1949341886599257</v>
+        <v>1.089004918819469E-05</v>
       </c>
       <c r="G7">
-        <v>3.765106465486745</v>
+        <v>0.2476353163504378</v>
       </c>
       <c r="H7">
-        <v>0.0001664781324763887</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>3.577416546058338</v>
+      </c>
+      <c r="I7">
+        <v>0.0003470069560616018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.05158627113362886</v>
+        <v>-0.07787178924719303</v>
       </c>
       <c r="C8">
-        <v>0.009175690948724899</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-5.622058482778079</v>
+        <v>0.008962409468301165</v>
       </c>
       <c r="E8">
-        <v>1.886953571172967E-08</v>
+        <v>-8.688711392021872</v>
       </c>
       <c r="F8">
-        <v>0.02053208289655751</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-2.512471403584584</v>
+        <v>0.01248819602300626</v>
       </c>
       <c r="H8">
-        <v>0.0119888821183991</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-6.235631559893394</v>
+      </c>
+      <c r="I8">
+        <v>4.499589589812558E-10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>4.154972234453322</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.8510205949935361</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>4.88234040268424</v>
+        <v>0.1643343117895808</v>
       </c>
       <c r="E9">
-        <v>1.048340799725267E-06</v>
+        <v>6.085156466170216</v>
       </c>
       <c r="F9">
-        <v>1.167324236095091</v>
+        <v>1.163775964485581E-09</v>
       </c>
       <c r="G9">
-        <v>3.559398585222946</v>
+        <v>0.2710680974375608</v>
       </c>
       <c r="H9">
-        <v>0.0003717050345077855</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>3.689109893244981</v>
+      </c>
+      <c r="I9">
+        <v>0.0002250400056729163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2506,61 +2617,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>5295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>4923</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>97484</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>80595</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-10290.95388350209</v>
+        <v>-9567.537760092964</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-1919.793256615122</v>
+        <v>-2121.343661144086</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>16742.32125377394</v>
+        <v>14892.38819789776</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.81344846373349</v>
+        <v>0.7782769491652914</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2571,7 +2682,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8126710819581402</v>
+        <v>0.7774407883681668</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2582,7 +2693,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>3855.586513230243</v>
+        <v>4258.687322288171</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2593,7 +2704,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>3908.182659294527</v>
+        <v>4310.700709326237</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2604,7 +2715,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.0291701453249266</v>
+        <v>41.70186242323294</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -2625,244 +2736,271 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.342658964443225</v>
+        <v>-4.4296279862931</v>
       </c>
       <c r="C2">
-        <v>0.4063955044199168</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-13.14645193250664</v>
+        <v>0.3756962574367033</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-11.7904501272265</v>
       </c>
       <c r="F2">
-        <v>0.5612090907312559</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>-9.519908092511002</v>
+        <v>0.415573930844739</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-10.65906125846002</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.709039747147089</v>
+        <v>-4.016512150888517</v>
       </c>
       <c r="C3">
-        <v>0.06889535290248923</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-39.32108092952681</v>
+        <v>0.08512383446479969</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-47.1843423894329</v>
       </c>
       <c r="F3">
-        <v>0.0791329106015102</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-34.23404657499593</v>
+        <v>0.1283892519610437</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-31.28386597428905</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-4.539678313528181</v>
+        <v>-4.983130048492587</v>
       </c>
       <c r="C4">
-        <v>0.1003455982058593</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-45.24043301047462</v>
+        <v>0.1460994598119297</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-34.10779242378617</v>
       </c>
       <c r="F4">
-        <v>0.1459679546909231</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-31.1005132814297</v>
+        <v>0.278823704772072</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-17.87197416577658</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.520521354733364</v>
+        <v>-2.21550201728977</v>
       </c>
       <c r="C5">
-        <v>0.03794089109818891</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>-66.43284545453598</v>
+        <v>0.03826538526500662</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-57.89833296976703</v>
       </c>
       <c r="F5">
-        <v>0.04512002190087188</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-55.86259156236488</v>
+        <v>0.04509544395408117</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-49.12917632091004</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.957258014762381</v>
+        <v>-3.345418058790918</v>
       </c>
       <c r="C6">
-        <v>0.06243693575821996</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-47.36391975118752</v>
+        <v>0.07121494651704484</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-46.97634727550085</v>
       </c>
       <c r="F6">
-        <v>0.06834704335569818</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-43.26826545183437</v>
+        <v>0.1147774762383458</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-29.14699092915978</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.6388570472887588</v>
+        <v>0.7198494911246508</v>
       </c>
       <c r="C7">
-        <v>0.079008726682325</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>8.085904862857094</v>
+        <v>0.08240733572617309</v>
       </c>
       <c r="E7">
-        <v>6.661338147750939E-16</v>
+        <v>8.735259850125479</v>
       </c>
       <c r="F7">
-        <v>0.09336622569538272</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>6.842485519047306</v>
+        <v>0.09934505394794292</v>
       </c>
       <c r="H7">
-        <v>7.783107491832197E-12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>7.245951987724058</v>
+      </c>
+      <c r="I7">
+        <v>4.294342659250105E-13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.2253874225052057</v>
+        <v>-0.132614717259584</v>
       </c>
       <c r="C8">
-        <v>0.00827368556948551</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>-27.24147788942638</v>
+        <v>0.004051506610461424</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-32.73219816972744</v>
       </c>
       <c r="F8">
-        <v>0.02795027849312859</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-8.063870367539122</v>
+        <v>0.004910876540030143</v>
       </c>
       <c r="H8">
-        <v>6.661338147750939E-16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-27.00428654204572</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>1.468873089191158</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.05487121891725866</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>26.76946344869975</v>
+        <v>0.04236434648239889</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>23.60475454083707</v>
       </c>
       <c r="F9">
-        <v>0.1052646865071707</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>13.95409170853416</v>
+        <v>0.09590311780426423</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>10.42718967740938</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2870,61 +3008,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>38829</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>32645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>63950</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>52873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-75418.7012644707</v>
+        <v>-63398.91231321533</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-13537.36842741692</v>
+        <v>-14284.48933712178</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>123762.6656741076</v>
+        <v>98228.8459521871</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8205038246423066</v>
+        <v>0.7746887317790117</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2935,7 +3073,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8203977501559276</v>
+        <v>0.7745625466488871</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -2946,7 +3084,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>27090.73685483385</v>
+        <v>28584.97867424355</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -2957,7 +3095,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>27159.27223618673</v>
+        <v>28652.12625011252</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2968,7 +3106,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.177048545115211</v>
+        <v>488.0235431490397</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
new run with more realistic pt prices
</commit_message>
<xml_diff>
--- a/input/estimation_results_splineGC_distVoT_knots2040_2.xlsx
+++ b/input/estimation_results_splineGC_distVoT_knots2040_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="29">
   <si>
     <t>Value</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>asc_rail</t>
-  </si>
-  <si>
-    <t>b_ac</t>
   </si>
   <si>
     <t>b_gc</t>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>.4E</t>
-  </si>
-  <si>
-    <t>Active bound</t>
   </si>
   <si>
     <t>mu_pt</t>
@@ -470,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,25 +498,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-1.672980411206608</v>
+        <v>-1.4543380311875</v>
       </c>
       <c r="C2">
-        <v>0.09837465124506885</v>
+        <v>0.1953582592304721</v>
       </c>
       <c r="D2">
-        <v>-17.00621440617781</v>
+        <v>-7.444466576003622</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>9.725553695716371E-14</v>
       </c>
       <c r="F2">
-        <v>0.06698565495354158</v>
+        <v>0.2380727903297765</v>
       </c>
       <c r="G2">
-        <v>-24.97520420404811</v>
+        <v>-6.108795671999991</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1.003857441617129E-09</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -530,22 +524,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-3.172365362002692</v>
+        <v>-3.007535382876413</v>
       </c>
       <c r="C3">
-        <v>0.03681075798972867</v>
+        <v>0.02028950872397102</v>
       </c>
       <c r="D3">
-        <v>-86.18038680126824</v>
+        <v>-148.231059893686</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.04271409608001418</v>
+        <v>0.02158715033881671</v>
       </c>
       <c r="G3">
-        <v>-74.26975291856952</v>
+        <v>-139.3206298965938</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -556,22 +550,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.277640166565115</v>
+        <v>-4.347986047100777</v>
       </c>
       <c r="C4">
-        <v>0.0805875730929403</v>
+        <v>0.06707934025576381</v>
       </c>
       <c r="D4">
-        <v>-65.489503703983</v>
+        <v>-64.81855710748698</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.09208822978042321</v>
+        <v>0.06467052558664635</v>
       </c>
       <c r="G4">
-        <v>-57.31069192174954</v>
+        <v>-67.23288557899987</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -582,22 +576,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.185409835006344</v>
+        <v>-2.573488019416509</v>
       </c>
       <c r="C5">
-        <v>0.02221264413057192</v>
+        <v>0.02835862126609918</v>
       </c>
       <c r="D5">
-        <v>-98.38584826551553</v>
+        <v>-90.74799494899777</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.02240191401144809</v>
+        <v>0.02818749379451045</v>
       </c>
       <c r="G5">
-        <v>-97.55460332048101</v>
+        <v>-91.29892987923954</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -608,22 +602,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.141938405479834</v>
+        <v>-1.622666332936903</v>
       </c>
       <c r="C6">
-        <v>0.03123343502117985</v>
+        <v>0.01634232314807116</v>
       </c>
       <c r="D6">
-        <v>-68.57838095705306</v>
+        <v>-99.29226819434311</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.03446794297528731</v>
+        <v>0.01926826364038507</v>
       </c>
       <c r="G6">
-        <v>-62.14291369274786</v>
+        <v>-84.21445560542863</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -634,22 +628,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.4432421580893682</v>
+        <v>-0.4473866552915687</v>
       </c>
       <c r="C7">
-        <v>0.04219750733705776</v>
+        <v>0.00627127267538952</v>
       </c>
       <c r="D7">
-        <v>10.50398912307585</v>
+        <v>-71.33905324309323</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.04928817490155355</v>
+        <v>0.009988796777323524</v>
       </c>
       <c r="G7">
-        <v>8.992870175750761</v>
+        <v>-44.78884346783607</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -660,25 +654,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.1395972114561939</v>
-      </c>
-      <c r="C8">
-        <v>0.001777925369090756</v>
-      </c>
-      <c r="D8">
-        <v>-78.5169129610794</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.004603949987866079</v>
-      </c>
-      <c r="G8">
-        <v>-30.32118329349986</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -686,7 +662,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>85496</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -694,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>85518</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -702,7 +678,10 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-166041.505415788</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -710,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>-166084.3154390672</v>
+        <v>-49229.68866923056</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -721,10 +700,10 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>-53448.43018347587</v>
+        <v>233623.633493115</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -732,7 +711,7 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>225271.7705111827</v>
+        <v>0.7035097426637187</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -743,10 +722,10 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.6781849626066287</v>
+        <v>0.7034736071204701</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -754,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.6781428153395525</v>
+        <v>98471.37733846111</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -765,10 +744,10 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>106910.8603669517</v>
+        <v>98527.51468768234</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -776,10 +755,10 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>106976.3557420653</v>
+        <v>671.6700928494116</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -787,17 +766,6 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>4323.442828912963</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
         <v>8</v>
       </c>
     </row>
@@ -808,336 +776,294 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-3.818346844050863</v>
+        <v>-2.854537699038605</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.242972776151441</v>
       </c>
       <c r="D2">
-        <v>0.2120296909587497</v>
+        <v>-11.74838491889074</v>
       </c>
       <c r="E2">
-        <v>-18.00854789150129</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.3064316570108107</v>
       </c>
       <c r="G2">
-        <v>0.2313566295003963</v>
+        <v>-9.315413840998483</v>
       </c>
       <c r="H2">
-        <v>-16.50416005928338</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-3.466486729244421</v>
+        <v>-2.759656958494784</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.02386790159392353</v>
       </c>
       <c r="D3">
-        <v>0.04148964468080995</v>
+        <v>-115.6221022461966</v>
       </c>
       <c r="E3">
-        <v>-83.55064874411329</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.0282681290343635</v>
       </c>
       <c r="G3">
-        <v>0.05483186862407576</v>
+        <v>-97.62432296598301</v>
       </c>
       <c r="H3">
-        <v>-63.22029170682583</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.28412159530715</v>
+        <v>-3.685704242393656</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.06643018045235914</v>
       </c>
       <c r="D4">
-        <v>0.09594694784847523</v>
+        <v>-55.48237589143513</v>
       </c>
       <c r="E4">
-        <v>-55.07336829152846</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.07127678250762824</v>
       </c>
       <c r="G4">
-        <v>0.1457321159920942</v>
+        <v>-51.70974492288848</v>
       </c>
       <c r="H4">
-        <v>-36.25914273826784</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.345845308152982</v>
+        <v>-2.478465176100142</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.02757006400698841</v>
       </c>
       <c r="D5">
-        <v>0.02371545650574094</v>
+        <v>-89.89696851889444</v>
       </c>
       <c r="E5">
-        <v>-98.91630412364653</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.02650136787499884</v>
       </c>
       <c r="G5">
-        <v>0.02361237688598294</v>
+        <v>-93.52216035755289</v>
       </c>
       <c r="H5">
-        <v>-99.34812236313029</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-3.009508142249753</v>
+        <v>-2.154007923832953</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.01802247378892805</v>
       </c>
       <c r="D6">
-        <v>0.03621806063523202</v>
+        <v>-119.5178835635899</v>
       </c>
       <c r="E6">
-        <v>-83.09412733497328</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.01845363172652725</v>
       </c>
       <c r="G6">
-        <v>0.0516124311368935</v>
+        <v>-116.7254205434559</v>
       </c>
       <c r="H6">
-        <v>-58.30975359923517</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.7157367362274738</v>
+        <v>-0.34356291342894</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.00645022040431675</v>
       </c>
       <c r="D7">
-        <v>0.04292927515119934</v>
+        <v>-53.26374788666348</v>
       </c>
       <c r="E7">
-        <v>16.67246264248833</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.009567035577530957</v>
       </c>
       <c r="G7">
-        <v>0.0517604712542244</v>
+        <v>-35.9111148531556</v>
       </c>
       <c r="H7">
-        <v>13.8278635971472</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1.395379999259929</v>
+      </c>
+      <c r="C8">
+        <v>0.02804791279234245</v>
+      </c>
+      <c r="D8">
+        <v>49.74986943202746</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.03225248320833496</v>
+      </c>
+      <c r="G8">
+        <v>43.26426558372174</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>-0.1530319204208467</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.002531391830031983</v>
-      </c>
-      <c r="E8">
-        <v>-60.45366766428777</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.003762704536853997</v>
-      </c>
-      <c r="H8">
-        <v>-40.67072471993695</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0.01933613189491461</v>
-      </c>
-      <c r="E9">
-        <v>51.71665178095931</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.03387254133351017</v>
-      </c>
-      <c r="H9">
-        <v>29.52243795804887</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>85496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>85518</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>-166041.505415788</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-166084.3154390672</v>
+        <v>-37876.10918075707</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-42154.94698063081</v>
+        <v>256330.7924700619</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>247858.7369168728</v>
+        <v>0.7718877031022412</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7461834558598246</v>
+        <v>0.7718455449684513</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1145,10 +1071,10 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7461352875545946</v>
+        <v>75766.21836151414</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1156,10 +1082,10 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>84325.89396126162</v>
+        <v>75831.71193560558</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1167,10 +1093,10 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>84400.74581853428</v>
+        <v>0.2842568825365753</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1178,17 +1104,6 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>672.3742929258788</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>
@@ -1199,7 +1114,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1233,25 +1148,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.562167911462441</v>
+        <v>-5.806419890123287</v>
       </c>
       <c r="C2">
-        <v>1.009460206027704</v>
+        <v>1.279224999870305</v>
       </c>
       <c r="D2">
-        <v>-5.510041780992988</v>
+        <v>-4.539013770612655</v>
       </c>
       <c r="E2">
-        <v>3.58748535322917E-08</v>
+        <v>5.651794545702415E-06</v>
       </c>
       <c r="F2">
-        <v>1.041649137950775</v>
+        <v>1.76474632054212</v>
       </c>
       <c r="G2">
-        <v>-5.339771050360426</v>
+        <v>-3.290229208886855</v>
       </c>
       <c r="H2">
-        <v>9.306403381259543E-08</v>
+        <v>0.001001058026410373</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1259,22 +1174,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-3.874770466325772</v>
+        <v>-2.887095089220199</v>
       </c>
       <c r="C3">
-        <v>0.08682543877342253</v>
+        <v>0.05501649113766344</v>
       </c>
       <c r="D3">
-        <v>-44.62713371869361</v>
+        <v>-52.47690337059206</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.1176308202507108</v>
+        <v>0.06865085137554926</v>
       </c>
       <c r="G3">
-        <v>-32.94009561497007</v>
+        <v>-42.05476015769367</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1285,22 +1200,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-6.18365992631436</v>
+        <v>-4.312098545966151</v>
       </c>
       <c r="C4">
-        <v>0.2321505306114727</v>
+        <v>0.1846467136723628</v>
       </c>
       <c r="D4">
-        <v>-26.63642383253191</v>
+        <v>-23.35323743490794</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.3134747229252904</v>
+        <v>0.2010137746111338</v>
       </c>
       <c r="G4">
-        <v>-19.72618356149914</v>
+        <v>-21.45175649931461</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1311,22 +1226,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.398805984487677</v>
+        <v>-3.853314853494675</v>
       </c>
       <c r="C5">
-        <v>0.07045698869847988</v>
+        <v>0.09052975422264718</v>
       </c>
       <c r="D5">
-        <v>-48.23944433720889</v>
+        <v>-42.56407063712892</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.0731178725682626</v>
+        <v>0.09837259226101552</v>
       </c>
       <c r="G5">
-        <v>-46.48392882758675</v>
+        <v>-39.17061414088323</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1337,22 +1252,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-2.99092739968023</v>
+        <v>-1.721758925581286</v>
       </c>
       <c r="C6">
-        <v>0.06938404315058853</v>
+        <v>0.03080662835453614</v>
       </c>
       <c r="D6">
-        <v>-43.10684797063257</v>
+        <v>-55.88923610096283</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.09781299543488969</v>
+        <v>0.0321772187264119</v>
       </c>
       <c r="G6">
-        <v>-30.57801661611697</v>
+        <v>-53.50863106661303</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1363,22 +1278,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>1.186767499615756</v>
+        <v>-0.5693738035062865</v>
       </c>
       <c r="C7">
-        <v>0.08435977603813884</v>
+        <v>0.02143591972248644</v>
       </c>
       <c r="D7">
-        <v>14.06793089492345</v>
+        <v>-26.56166895927536</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.1067343984295755</v>
+        <v>0.03327392691124373</v>
       </c>
       <c r="G7">
-        <v>11.11888498063535</v>
+        <v>-17.11171047003434</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1386,25 +1301,25 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>-0.1426630346561793</v>
+        <v>1.279614610828804</v>
       </c>
       <c r="C8">
-        <v>0.004867241824864233</v>
+        <v>0.04765950259671289</v>
       </c>
       <c r="D8">
-        <v>-29.31085813887185</v>
+        <v>26.84909705534903</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.009703332617792557</v>
+        <v>0.05906897631969113</v>
       </c>
       <c r="G8">
-        <v>-14.70247803260754</v>
+        <v>21.66305716732446</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1412,28 +1327,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>1.017374512202527</v>
-      </c>
-      <c r="C9">
-        <v>0.03580135398466828</v>
-      </c>
-      <c r="D9">
-        <v>28.41720770220622</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.05234822034042511</v>
-      </c>
-      <c r="G9">
-        <v>19.43474879540221</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1441,7 +1338,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>22969</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1449,7 +1346,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>22973</v>
+        <v>62527</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1457,7 +1354,10 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>62545</v>
+        <v>-44602.81150439663</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1465,10 +1365,10 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-44610.59514499285</v>
+        <v>-10121.05722577291</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1476,10 +1376,10 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-11326.9880144851</v>
+        <v>68963.50855724743</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1487,7 +1387,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>66567.2142610155</v>
+        <v>0.7730847701209318</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1498,10 +1398,10 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7460919770814478</v>
+        <v>0.7729278293415527</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1509,10 +1409,10 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7459126474855524</v>
+        <v>20256.11445154582</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1520,10 +1420,10 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>22669.9760289702</v>
+        <v>20312.40775686365</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1531,10 +1431,10 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>22734.31262810854</v>
+        <v>0.09507242521343873</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1542,17 +1442,6 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.1506166934773418</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>
@@ -1563,336 +1452,294 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-7.233566997328035</v>
+        <v>-4.74246661852334</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>12.61171340273545</v>
       </c>
       <c r="D2">
-        <v>9.713305320796357</v>
+        <v>-0.3760366626706496</v>
       </c>
       <c r="E2">
-        <v>-0.7447070547489989</v>
+        <v>0.7068896400417715</v>
       </c>
       <c r="F2">
-        <v>0.4564488334233063</v>
+        <v>0.3693969669136684</v>
       </c>
       <c r="G2">
-        <v>0.1914988489903077</v>
+        <v>-12.83840162020524</v>
       </c>
       <c r="H2">
-        <v>-37.77342284545087</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-0.4618166150392248</v>
+        <v>0.1667771368666988</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.04741987721976725</v>
       </c>
       <c r="D3">
-        <v>0.0851710807783144</v>
+        <v>3.517030128394698</v>
       </c>
       <c r="E3">
-        <v>-5.422223257225697</v>
+        <v>0.0004364042441813432</v>
       </c>
       <c r="F3">
-        <v>5.886230058926856E-08</v>
+        <v>0.04755542055797623</v>
       </c>
       <c r="G3">
-        <v>0.09424677693644623</v>
+        <v>3.507005824149444</v>
       </c>
       <c r="H3">
-        <v>-4.900078602694745</v>
-      </c>
-      <c r="I3">
-        <v>9.579832092043716E-07</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0.0004531792296664783</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-3.11288913405289</v>
+        <v>-0.8348064096191902</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.1524735028349067</v>
       </c>
       <c r="D4">
-        <v>0.2699019422146252</v>
+        <v>-5.475091698543133</v>
       </c>
       <c r="E4">
-        <v>-11.5334076832153</v>
+        <v>4.372851103440212E-08</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.1544176956144691</v>
       </c>
       <c r="G4">
-        <v>0.3827514835838884</v>
+        <v>-5.406157670578318</v>
       </c>
       <c r="H4">
-        <v>-8.132925063817895</v>
-      </c>
-      <c r="I4">
-        <v>4.440892098500626E-16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>6.439111821521237E-08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-1.122447474876091</v>
+        <v>-1.502894602428474</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.09708100976493735</v>
       </c>
       <c r="D5">
-        <v>0.07636771751165398</v>
+        <v>-15.4808299384961</v>
       </c>
       <c r="E5">
-        <v>-14.69793142246004</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.08557234433108654</v>
       </c>
       <c r="G5">
-        <v>0.06794155557354124</v>
+        <v>-17.5628541461205</v>
       </c>
       <c r="H5">
-        <v>-16.52077974077489</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-0.8404783913427564</v>
+        <v>0.2062420147794096</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.05224829649097956</v>
       </c>
       <c r="D6">
-        <v>0.09213149164789218</v>
+        <v>3.947344289301689</v>
       </c>
       <c r="E6">
-        <v>-9.122596153711413</v>
+        <v>7.902287978400757E-05</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.05132574623558078</v>
       </c>
       <c r="G6">
-        <v>0.1259856593745364</v>
+        <v>4.018295493119115</v>
       </c>
       <c r="H6">
-        <v>-6.67122270515044</v>
-      </c>
-      <c r="I6">
-        <v>2.536815202347498E-11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>5.862065542494577E-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.6230555544287325</v>
+        <v>-0.4581824928620072</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.02882574419890533</v>
       </c>
       <c r="D7">
-        <v>0.1034534501122434</v>
+        <v>-15.89490594589425</v>
       </c>
       <c r="E7">
-        <v>6.022569124110783</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1.716700115395042E-09</v>
+        <v>0.03695071435899409</v>
       </c>
       <c r="G7">
-        <v>0.1062863986339531</v>
+        <v>-12.39982773839072</v>
       </c>
       <c r="H7">
-        <v>5.862044085005792</v>
-      </c>
-      <c r="I7">
-        <v>4.572035861016843E-09</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>2.020061915783203</v>
+      </c>
+      <c r="C8">
+        <v>0.1422409256468261</v>
+      </c>
+      <c r="D8">
+        <v>14.20169270269563</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.1475376855704364</v>
+      </c>
+      <c r="G8">
+        <v>13.6918368210324</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>-0.1605231608246017</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.007533943685942933</v>
-      </c>
-      <c r="E8">
-        <v>-21.30665790933781</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.01173981340637617</v>
-      </c>
-      <c r="H8">
-        <v>-13.67339967579193</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0.05016420477456989</v>
-      </c>
-      <c r="E9">
-        <v>19.93453308975681</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.07510141093945774</v>
-      </c>
-      <c r="H9">
-        <v>13.31532906626934</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>3693</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>81803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>81825</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>-7168.673002960919</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-7168.673002960919</v>
+        <v>-3591.359750736333</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-4196.470925158025</v>
+        <v>7154.626504449172</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>5944.404155605787</v>
+        <v>0.4990202860064934</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.4146097996903008</v>
+        <v>0.4980438151872625</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1900,10 +1747,10 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.4134938330397512</v>
+        <v>7196.719501472666</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1911,10 +1758,10 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>8408.94185031605</v>
+        <v>7240.218862376633</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1922,10 +1769,10 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>8458.65540563487</v>
+        <v>0.03735699109160988</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1933,17 +1780,6 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>22.95556482222339</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>
@@ -1954,336 +1790,294 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-5.15428519278747</v>
+        <v>-5.835578194899073</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.499139466241748</v>
       </c>
       <c r="D2">
-        <v>1.030869407664259</v>
+        <v>-3.892618616417667</v>
       </c>
       <c r="E2">
-        <v>-4.999940006432079</v>
+        <v>9.916798574938213E-05</v>
       </c>
       <c r="F2">
-        <v>5.734815577973507E-07</v>
+        <v>2.331154261185054</v>
       </c>
       <c r="G2">
-        <v>1.063478147455382</v>
+        <v>-2.503299885410641</v>
       </c>
       <c r="H2">
-        <v>-4.84663009307741</v>
-      </c>
-      <c r="I2">
-        <v>1.255762537732963E-06</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0.01230412395941971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-4.087511920259394</v>
+        <v>-3.226522896420422</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05422592782348212</v>
       </c>
       <c r="D3">
-        <v>0.1088970626018388</v>
+        <v>-59.50147882989659</v>
       </c>
       <c r="E3">
-        <v>-37.53555718214913</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.0596107492503136</v>
       </c>
       <c r="G3">
-        <v>0.1401789229288025</v>
+        <v>-54.12652813457881</v>
       </c>
       <c r="H3">
-        <v>-29.15924758770947</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-6.895030542932053</v>
+        <v>-4.985405141285787</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.2696189395294016</v>
       </c>
       <c r="D4">
-        <v>0.3634403564761442</v>
+        <v>-18.49055986195708</v>
       </c>
       <c r="E4">
-        <v>-18.97156003748482</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.2784066873263824</v>
       </c>
       <c r="G4">
-        <v>0.524275958647925</v>
+        <v>-17.9069159191614</v>
       </c>
       <c r="H4">
-        <v>-13.15152913117341</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.258752699669295</v>
+        <v>-2.617709813782954</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.05874919351518181</v>
       </c>
       <c r="D5">
-        <v>0.04975895003499979</v>
+        <v>-44.55737444474863</v>
       </c>
       <c r="E5">
-        <v>-45.39389794359644</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.05579524516944926</v>
       </c>
       <c r="G5">
-        <v>0.04642912899257431</v>
+        <v>-46.91636009185033</v>
       </c>
       <c r="H5">
-        <v>-48.64947391174516</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-3.753755439077343</v>
+        <v>-2.756860708404343</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.04762821231952182</v>
       </c>
       <c r="D6">
-        <v>0.09876368824433451</v>
+        <v>-57.8829348015307</v>
       </c>
       <c r="E6">
-        <v>-38.00744490010147</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.04969855702646427</v>
       </c>
       <c r="G6">
-        <v>0.1454000558498358</v>
+        <v>-55.47164491991843</v>
       </c>
       <c r="H6">
-        <v>-25.81674000836763</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.9905134710247595</v>
+        <v>-0.5358635868280535</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.0180450033153946</v>
       </c>
       <c r="D7">
-        <v>0.1165443909943353</v>
+        <v>-29.69595391378489</v>
       </c>
       <c r="E7">
-        <v>8.499023098184999</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.02249906115919606</v>
       </c>
       <c r="G7">
-        <v>0.1438286446706847</v>
+        <v>-23.81715321525891</v>
       </c>
       <c r="H7">
-        <v>6.88676079297469</v>
-      </c>
-      <c r="I7">
-        <v>5.70765656959793E-12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1.374307784590379</v>
+      </c>
+      <c r="C8">
+        <v>0.06282510668033821</v>
+      </c>
+      <c r="D8">
+        <v>21.8751365052673</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.07173494270110027</v>
+      </c>
+      <c r="G8">
+        <v>19.15813594940391</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>-0.2620702823242717</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.01143039230226287</v>
-      </c>
-      <c r="E8">
-        <v>-22.92749674675556</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.01803292406051982</v>
-      </c>
-      <c r="H8">
-        <v>-14.53287783194475</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0.04870775357144485</v>
-      </c>
-      <c r="E9">
-        <v>20.53061220598469</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.09497672273616414</v>
-      </c>
-      <c r="H9">
-        <v>10.52889561980255</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>21276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>21284</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>64220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>64234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>-41323.02993662904</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-41338.59721782148</v>
+        <v>-6266.723004672147</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-7020.168444799745</v>
+        <v>70112.61386391379</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>68636.85754604347</v>
+        <v>0.8483479305781187</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.8301788421167499</v>
+        <v>0.8481785335128325</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2291,10 +2085,10 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.8299853183752972</v>
+        <v>12547.44600934429</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2302,10 +2096,10 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>14056.33688959949</v>
+        <v>12603.20335403533</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2313,10 +2107,10 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>14120.06257676522</v>
+        <v>0.2661193540644802</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2324,17 +2118,6 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>177.9766714558397</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>
@@ -2345,336 +2128,294 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-2.56527896921774</v>
+        <v>-1.885105874803393</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.3042635819869521</v>
       </c>
       <c r="D2">
-        <v>0.2975998408780923</v>
+        <v>-6.195634267147464</v>
       </c>
       <c r="E2">
-        <v>-8.619893618385944</v>
+        <v>5.805078640008787E-10</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.3490462953727916</v>
       </c>
       <c r="G2">
-        <v>0.3684566167393651</v>
+        <v>-5.400733082670437</v>
       </c>
       <c r="H2">
-        <v>-6.962227987433159</v>
-      </c>
-      <c r="I2">
-        <v>3.349320820689172E-12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>6.636911531465728E-08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-4.552613433800848</v>
+        <v>-3.486204396878051</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.1434508141468472</v>
       </c>
       <c r="D3">
-        <v>0.2786932846654471</v>
+        <v>-24.30243716364903</v>
       </c>
       <c r="E3">
-        <v>-16.33556918770382</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.1474178095779123</v>
       </c>
       <c r="G3">
-        <v>0.4041507488752643</v>
+        <v>-23.64846151804707</v>
       </c>
       <c r="H3">
-        <v>-11.26464183592531</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-5.770148450447874</v>
+        <v>-3.856950213437547</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.2760081731023992</v>
       </c>
       <c r="D4">
-        <v>0.5620648929450079</v>
+        <v>-13.97404348604784</v>
       </c>
       <c r="E4">
-        <v>-10.265982670105</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.2829799397274805</v>
       </c>
       <c r="G4">
-        <v>0.8711637915431425</v>
+        <v>-13.62976547790604</v>
       </c>
       <c r="H4">
-        <v>-6.623494349124496</v>
-      </c>
-      <c r="I4">
-        <v>3.508060508750077E-11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-3.603596977143348</v>
+        <v>-3.064836693448962</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.1664802065295579</v>
       </c>
       <c r="D5">
-        <v>0.1751034577406484</v>
+        <v>-18.40961611796662</v>
       </c>
       <c r="E5">
-        <v>-20.57981620489047</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.1683278130650497</v>
       </c>
       <c r="G5">
-        <v>0.2352023450792066</v>
+        <v>-18.20754774651868</v>
       </c>
       <c r="H5">
-        <v>-15.32126295734765</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-3.481006697370505</v>
+        <v>-2.49571742596636</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.08298362474719508</v>
       </c>
       <c r="D6">
-        <v>0.1897212314789268</v>
+        <v>-30.07481817731416</v>
       </c>
       <c r="E6">
-        <v>-18.34800812874313</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.0824749839471154</v>
       </c>
       <c r="G6">
-        <v>0.2607918969731022</v>
+        <v>-30.26029598946831</v>
       </c>
       <c r="H6">
-        <v>-13.34783303382134</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.8858946781004471</v>
+        <v>-0.1900954626373776</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.0163885159901625</v>
       </c>
       <c r="D7">
-        <v>0.2013991355605487</v>
+        <v>-11.59930909860819</v>
       </c>
       <c r="E7">
-        <v>4.398701492112966</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1.089004918819469E-05</v>
+        <v>0.02037615802548374</v>
       </c>
       <c r="G7">
-        <v>0.2476353163504378</v>
+        <v>-9.329308420146331</v>
       </c>
       <c r="H7">
-        <v>3.577416546058338</v>
-      </c>
-      <c r="I7">
-        <v>0.0003470069560616018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1.499198047612213</v>
+      </c>
+      <c r="C8">
+        <v>0.1647104694908583</v>
+      </c>
+      <c r="D8">
+        <v>9.10202036486467</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.1689821771003408</v>
+      </c>
+      <c r="G8">
+        <v>8.871930006689384</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>-0.07787178924719303</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.008962409468301165</v>
-      </c>
-      <c r="E8">
-        <v>-8.688711392021872</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.01248819602300626</v>
-      </c>
-      <c r="H8">
-        <v>-6.235631559893394</v>
-      </c>
-      <c r="I8">
-        <v>4.499589589812558E-10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0.1643343117895808</v>
-      </c>
-      <c r="E9">
-        <v>6.085156466170216</v>
-      </c>
-      <c r="F9">
-        <v>1.163775964485581E-09</v>
-      </c>
-      <c r="G9">
-        <v>0.2710680974375608</v>
-      </c>
-      <c r="H9">
-        <v>3.689109893244981</v>
-      </c>
-      <c r="I9">
-        <v>0.0002250400056729163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>4923</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>4923</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>80573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>80595</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>-9567.537760092964</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-9567.537760092964</v>
+        <v>-1935.128891630009</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-2121.343661144086</v>
+        <v>15264.81773692591</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>14892.38819789776</v>
+        <v>0.7977401354294518</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7782769491652914</v>
+        <v>0.7970084947319677</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2682,10 +2423,10 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7774407883681668</v>
+        <v>3884.257783260019</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2693,10 +2434,10 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>4258.687322288171</v>
+        <v>3929.769496918326</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2704,10 +2445,10 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>4310.700709326237</v>
+        <v>0.04380609033265895</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2715,17 +2456,6 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>41.70186242323294</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>
@@ -2736,336 +2466,294 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-4.4296279862931</v>
+        <v>-3.10983193692737</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.4114091281853129</v>
       </c>
       <c r="D2">
-        <v>0.3756962574367033</v>
+        <v>-7.55897651236993</v>
       </c>
       <c r="E2">
-        <v>-11.7904501272265</v>
+        <v>4.063416270128073E-14</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.5240061746062628</v>
       </c>
       <c r="G2">
-        <v>0.415573930844739</v>
+        <v>-5.934723840351866</v>
       </c>
       <c r="H2">
-        <v>-10.65906125846002</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2.943405075228611E-09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-4.016512150888517</v>
+        <v>-3.351646566665337</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.04746624945321478</v>
       </c>
       <c r="D3">
-        <v>0.08512383446479969</v>
+        <v>-70.61115224553176</v>
       </c>
       <c r="E3">
-        <v>-47.1843423894329</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.05497707891066431</v>
       </c>
       <c r="G3">
-        <v>0.1283892519610437</v>
+        <v>-60.96443523512111</v>
       </c>
       <c r="H3">
-        <v>-31.28386597428905</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-4.983130048492587</v>
+        <v>-3.750468896520653</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.09460496509484984</v>
       </c>
       <c r="D4">
-        <v>0.1460994598119297</v>
+        <v>-39.64346789579676</v>
       </c>
       <c r="E4">
-        <v>-34.10779242378617</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.1002483413496487</v>
       </c>
       <c r="G4">
-        <v>0.278823704772072</v>
+        <v>-37.4117800457134</v>
       </c>
       <c r="H4">
-        <v>-17.87197416577658</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-2.21550201728977</v>
+        <v>-2.135244635753526</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.03968831094719418</v>
       </c>
       <c r="D5">
-        <v>0.03826538526500662</v>
+        <v>-53.80034032172588</v>
       </c>
       <c r="E5">
-        <v>-57.89833296976703</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.03750238943386355</v>
       </c>
       <c r="G5">
-        <v>0.04509544395408117</v>
+        <v>-56.93622907732549</v>
       </c>
       <c r="H5">
-        <v>-49.12917632091004</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-3.345418058790918</v>
+        <v>-2.575907077835372</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.0342279405873931</v>
       </c>
       <c r="D6">
-        <v>0.07121494651704484</v>
+        <v>-75.25743686677237</v>
       </c>
       <c r="E6">
-        <v>-46.97634727550085</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.03454693728733648</v>
       </c>
       <c r="G6">
-        <v>0.1147774762383458</v>
+        <v>-74.56253086665357</v>
       </c>
       <c r="H6">
-        <v>-29.14699092915978</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.7198494911246508</v>
+        <v>-0.2665266390021757</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.007913643610343059</v>
       </c>
       <c r="D7">
-        <v>0.08240733572617309</v>
+        <v>-33.67938362220758</v>
       </c>
       <c r="E7">
-        <v>8.735259850125479</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.01118263790195849</v>
       </c>
       <c r="G7">
-        <v>0.09934505394794292</v>
+        <v>-23.83396845528703</v>
       </c>
       <c r="H7">
-        <v>7.245951987724058</v>
-      </c>
-      <c r="I7">
-        <v>4.294342659250105E-13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1.264410625041325</v>
+      </c>
+      <c r="C8">
+        <v>0.04328026296833379</v>
+      </c>
+      <c r="D8">
+        <v>29.21448573374975</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.04698036286311982</v>
+      </c>
+      <c r="G8">
+        <v>26.91359853318424</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>-0.132614717259584</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.004051506610461424</v>
-      </c>
-      <c r="E8">
-        <v>-32.73219816972744</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.004910876540030143</v>
-      </c>
-      <c r="H8">
-        <v>-27.00428654204572</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0.04236434648239889</v>
-      </c>
-      <c r="E9">
-        <v>23.60475454083707</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.09590311780426423</v>
-      </c>
-      <c r="H9">
-        <v>10.42718967740938</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>32635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>32645</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>52861</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>52873</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>-63379.45321172476</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-63398.91231321533</v>
+        <v>-12806.93513871557</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>-14284.48933712178</v>
+        <v>101145.0361460184</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>98228.8459521871</v>
+        <v>0.7979323820302953</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.7746887317790117</v>
+        <v>0.7978219361421521</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3073,10 +2761,10 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.7745625466488871</v>
+        <v>25627.87027743115</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3084,10 +2772,10 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>28584.97867424355</v>
+        <v>25686.62226170863</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3095,10 +2783,10 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>28652.12625011252</v>
+        <v>0.1239333268326568</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3106,17 +2794,6 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>488.0235431490397</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>

</xml_diff>